<commit_message>
GDE-9543 - Initial commit
</commit_message>
<xml_diff>
--- a/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Base_Rate/BaseRates_Files_16MAR2020/TL_Transformed_Data_BaseRate.xlsx
+++ b/DataSet/NewUATDeals_DataSet/Transformation_Layer/TL_Base_Rate/BaseRates_Files_16MAR2020/TL_Transformed_Data_BaseRate.xlsx
@@ -387,7 +387,7 @@
     <outlinePr summaryBelow="0" summaryRight="0"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H11" sqref="H11"/>
@@ -509,7 +509,7 @@
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>0.58510</t>
+          <t>0.5851</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -558,6 +558,81 @@
         </is>
       </c>
       <c r="O2" t="inlineStr">
+        <is>
+          <t>AUD,EUR</t>
+        </is>
+      </c>
+    </row>
+    <row r="3">
+      <c r="A3" t="n">
+        <v>2</v>
+      </c>
+      <c r="B3" t="inlineStr">
+        <is>
+          <t>BANKBILL</t>
+        </is>
+      </c>
+      <c r="C3" t="inlineStr">
+        <is>
+          <t>AUD</t>
+        </is>
+      </c>
+      <c r="D3" t="inlineStr">
+        <is>
+          <t>0.6433</t>
+        </is>
+      </c>
+      <c r="E3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="F3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="G3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="H3" t="inlineStr">
+        <is>
+          <t>2020-03-16</t>
+        </is>
+      </c>
+      <c r="I3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="J3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="K3" t="inlineStr">
+        <is>
+          <t>003M</t>
+        </is>
+      </c>
+      <c r="L3" t="inlineStr">
+        <is>
+          <t>DEPOSIT</t>
+        </is>
+      </c>
+      <c r="M3" t="inlineStr">
+        <is>
+          <t>COMRLENDING</t>
+        </is>
+      </c>
+      <c r="N3" t="inlineStr">
+        <is>
+          <t>null</t>
+        </is>
+      </c>
+      <c r="O3" t="inlineStr">
         <is>
           <t>AUD,EUR</t>
         </is>

</xml_diff>